<commit_message>
Updated the venn diagram (not finished) and the 528 ok pairs (not finished of finding duplicates)
</commit_message>
<xml_diff>
--- a/results/common_ok_pairs_fixed_nicadfse13_2016-07-17.xlsx
+++ b/results/common_ok_pairs_fixed_nicadfse13_2016-07-17.xlsx
@@ -31,7 +31,7 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11127" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11285" uniqueCount="311">
   <si>
     <t>stackoverflow_formatted/6236324_0.java</t>
   </si>
@@ -976,6 +976,9 @@
   <si>
     <t>Count of Classifications</t>
   </si>
+  <si>
+    <t>duplicate</t>
+  </si>
 </sst>
 </file>
 
@@ -1069,7 +1072,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1102,6 +1105,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1110,7 +1118,18 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
@@ -9373,7 +9392,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="X1:Y8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -9692,10 +9711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z529"/>
+  <dimension ref="A1:Z550"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A499" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:S529"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24964,52 +24983,53 @@
       </c>
     </row>
     <row r="302" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B302" t="s">
+      <c r="B302" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="C302" s="5">
+      <c r="C302" s="33">
         <v>0.83333333333333304</v>
       </c>
-      <c r="D302" t="s">
+      <c r="D302" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="E302">
+      <c r="E302" s="17">
         <v>5</v>
       </c>
-      <c r="F302">
+      <c r="F302" s="17">
         <v>10</v>
       </c>
-      <c r="G302" t="s">
+      <c r="G302" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="H302">
+      <c r="H302" s="17">
         <v>85</v>
       </c>
-      <c r="I302">
+      <c r="I302" s="17">
         <v>91</v>
       </c>
-      <c r="J302" t="s">
+      <c r="J302" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="K302">
+      <c r="K302" s="17">
         <v>3</v>
       </c>
-      <c r="L302">
+      <c r="L302" s="17">
         <v>9</v>
       </c>
-      <c r="M302" t="s">
+      <c r="M302" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="N302">
+      <c r="N302" s="17">
         <v>82</v>
       </c>
-      <c r="O302">
+      <c r="O302" s="17">
         <v>90</v>
       </c>
-      <c r="Q302" t="s">
+      <c r="P302" s="17"/>
+      <c r="Q302" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="R302" s="18" t="s">
+      <c r="R302" s="34" t="s">
         <v>272</v>
       </c>
     </row>
@@ -36869,7 +36889,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="529" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>248</v>
       </c>
@@ -36922,8 +36942,1062 @@
         <v>250</v>
       </c>
     </row>
+    <row r="533" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A533" s="6"/>
+      <c r="B533" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C533" s="7">
+        <v>1</v>
+      </c>
+      <c r="D533" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E533" s="6">
+        <v>50</v>
+      </c>
+      <c r="F533" s="6">
+        <v>66</v>
+      </c>
+      <c r="G533" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H533" s="6">
+        <v>47</v>
+      </c>
+      <c r="I533" s="6">
+        <v>63</v>
+      </c>
+      <c r="J533" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="K533" s="6">
+        <v>51</v>
+      </c>
+      <c r="L533" s="6">
+        <v>63</v>
+      </c>
+      <c r="M533" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="N533" s="6">
+        <v>48</v>
+      </c>
+      <c r="O533" s="6">
+        <v>60</v>
+      </c>
+      <c r="P533" s="6"/>
+      <c r="Q533" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="R533" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="S533" s="6"/>
+      <c r="T533" s="6"/>
+      <c r="U533" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="534" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A534" s="6"/>
+      <c r="B534" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C534" s="7">
+        <v>1</v>
+      </c>
+      <c r="D534" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E534" s="6">
+        <v>50</v>
+      </c>
+      <c r="F534" s="6">
+        <v>66</v>
+      </c>
+      <c r="G534" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H534" s="6">
+        <v>51</v>
+      </c>
+      <c r="I534" s="6">
+        <v>67</v>
+      </c>
+      <c r="J534" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="K534" s="6">
+        <v>51</v>
+      </c>
+      <c r="L534" s="6">
+        <v>63</v>
+      </c>
+      <c r="M534" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="N534" s="6">
+        <v>52</v>
+      </c>
+      <c r="O534" s="6">
+        <v>64</v>
+      </c>
+      <c r="P534" s="6"/>
+      <c r="Q534" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="R534" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="S534" s="6"/>
+      <c r="T534" s="6"/>
+      <c r="U534" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="535" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A535" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B535" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C535" s="7">
+        <v>0.78571428571428503</v>
+      </c>
+      <c r="D535" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E535" s="6">
+        <v>124</v>
+      </c>
+      <c r="F535" s="6">
+        <v>137</v>
+      </c>
+      <c r="G535" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H535" s="6">
+        <v>132</v>
+      </c>
+      <c r="I535" s="6">
+        <v>145</v>
+      </c>
+      <c r="J535" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K535" s="6">
+        <v>114</v>
+      </c>
+      <c r="L535" s="6">
+        <v>134</v>
+      </c>
+      <c r="M535" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N535" s="6">
+        <v>122</v>
+      </c>
+      <c r="O535" s="6">
+        <v>142</v>
+      </c>
+      <c r="P535" s="6"/>
+      <c r="Q535" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R535" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="S535" s="6"/>
+      <c r="T535" s="6"/>
+      <c r="U535" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="536" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A536" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B536" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C536" s="7">
+        <v>0.78571428571428503</v>
+      </c>
+      <c r="D536" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E536" s="6">
+        <v>124</v>
+      </c>
+      <c r="F536" s="6">
+        <v>137</v>
+      </c>
+      <c r="G536" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H536" s="6">
+        <v>132</v>
+      </c>
+      <c r="I536" s="6">
+        <v>145</v>
+      </c>
+      <c r="J536" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K536" s="6">
+        <v>77</v>
+      </c>
+      <c r="L536" s="6">
+        <v>134</v>
+      </c>
+      <c r="M536" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N536" s="6">
+        <v>85</v>
+      </c>
+      <c r="O536" s="6">
+        <v>142</v>
+      </c>
+      <c r="P536" s="6"/>
+      <c r="Q536" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R536" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="S536" s="6"/>
+      <c r="T536" s="6"/>
+      <c r="U536" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="537" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A537" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B537" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C537" s="7">
+        <v>0.78571428571428503</v>
+      </c>
+      <c r="D537" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E537" s="6">
+        <v>124</v>
+      </c>
+      <c r="F537" s="6">
+        <v>137</v>
+      </c>
+      <c r="G537" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H537" s="6">
+        <v>132</v>
+      </c>
+      <c r="I537" s="6">
+        <v>145</v>
+      </c>
+      <c r="J537" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K537" s="6">
+        <v>114</v>
+      </c>
+      <c r="L537" s="6">
+        <v>134</v>
+      </c>
+      <c r="M537" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N537" s="6">
+        <v>122</v>
+      </c>
+      <c r="O537" s="6">
+        <v>142</v>
+      </c>
+      <c r="P537" s="6"/>
+      <c r="Q537" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R537" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="S537" s="6"/>
+      <c r="T537" s="6"/>
+      <c r="U537" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="538" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A538" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B538" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C538" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="D538" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E538" s="6">
+        <v>124</v>
+      </c>
+      <c r="F538" s="6">
+        <v>137</v>
+      </c>
+      <c r="G538" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H538" s="6">
+        <v>132</v>
+      </c>
+      <c r="I538" s="6">
+        <v>145</v>
+      </c>
+      <c r="J538" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K538" s="6">
+        <v>77</v>
+      </c>
+      <c r="L538" s="6">
+        <v>134</v>
+      </c>
+      <c r="M538" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N538" s="6">
+        <v>85</v>
+      </c>
+      <c r="O538" s="6">
+        <v>142</v>
+      </c>
+      <c r="P538" s="6"/>
+      <c r="Q538" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="R538" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="S538" s="6"/>
+      <c r="T538" s="6"/>
+      <c r="U538" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="539" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A539" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B539" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C539" s="7">
+        <v>1</v>
+      </c>
+      <c r="D539" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E539" s="6">
+        <v>114</v>
+      </c>
+      <c r="F539" s="6">
+        <v>123</v>
+      </c>
+      <c r="G539" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H539" s="6">
+        <v>122</v>
+      </c>
+      <c r="I539" s="6">
+        <v>131</v>
+      </c>
+      <c r="J539" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K539" s="6">
+        <v>114</v>
+      </c>
+      <c r="L539" s="6">
+        <v>134</v>
+      </c>
+      <c r="M539" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N539" s="6">
+        <v>122</v>
+      </c>
+      <c r="O539" s="6">
+        <v>142</v>
+      </c>
+      <c r="P539" s="6"/>
+      <c r="Q539" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R539" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="S539" s="6"/>
+      <c r="T539" s="6"/>
+      <c r="U539" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="540" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A540" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B540" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C540" s="7">
+        <v>1</v>
+      </c>
+      <c r="D540" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E540" s="6">
+        <v>114</v>
+      </c>
+      <c r="F540" s="6">
+        <v>123</v>
+      </c>
+      <c r="G540" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H540" s="6">
+        <v>122</v>
+      </c>
+      <c r="I540" s="6">
+        <v>131</v>
+      </c>
+      <c r="J540" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K540" s="6">
+        <v>77</v>
+      </c>
+      <c r="L540" s="6">
+        <v>134</v>
+      </c>
+      <c r="M540" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N540" s="6">
+        <v>85</v>
+      </c>
+      <c r="O540" s="6">
+        <v>142</v>
+      </c>
+      <c r="P540" s="6"/>
+      <c r="Q540" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R540" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="S540" s="6"/>
+      <c r="T540" s="6"/>
+      <c r="U540" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="541" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A541" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B541" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C541" s="7">
+        <v>1</v>
+      </c>
+      <c r="D541" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E541" s="6">
+        <v>114</v>
+      </c>
+      <c r="F541" s="6">
+        <v>123</v>
+      </c>
+      <c r="G541" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H541" s="6">
+        <v>122</v>
+      </c>
+      <c r="I541" s="6">
+        <v>131</v>
+      </c>
+      <c r="J541" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K541" s="6">
+        <v>114</v>
+      </c>
+      <c r="L541" s="6">
+        <v>134</v>
+      </c>
+      <c r="M541" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N541" s="6">
+        <v>122</v>
+      </c>
+      <c r="O541" s="6">
+        <v>142</v>
+      </c>
+      <c r="P541" s="6"/>
+      <c r="Q541" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R541" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="S541" s="6"/>
+      <c r="T541" s="6"/>
+      <c r="U541" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="542" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A542" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B542" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C542" s="7">
+        <v>1</v>
+      </c>
+      <c r="D542" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E542" s="6">
+        <v>114</v>
+      </c>
+      <c r="F542" s="6">
+        <v>123</v>
+      </c>
+      <c r="G542" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H542" s="6">
+        <v>122</v>
+      </c>
+      <c r="I542" s="6">
+        <v>131</v>
+      </c>
+      <c r="J542" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K542" s="6">
+        <v>77</v>
+      </c>
+      <c r="L542" s="6">
+        <v>134</v>
+      </c>
+      <c r="M542" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N542" s="6">
+        <v>85</v>
+      </c>
+      <c r="O542" s="6">
+        <v>142</v>
+      </c>
+      <c r="P542" s="6"/>
+      <c r="Q542" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R542" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="S542" s="6"/>
+      <c r="T542" s="6"/>
+      <c r="U542" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="543" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A543" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B543" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C543" s="7">
+        <v>1</v>
+      </c>
+      <c r="D543" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E543" s="6">
+        <v>93</v>
+      </c>
+      <c r="F543" s="6">
+        <v>110</v>
+      </c>
+      <c r="G543" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H543" s="6">
+        <v>101</v>
+      </c>
+      <c r="I543" s="6">
+        <v>118</v>
+      </c>
+      <c r="J543" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K543" s="6">
+        <v>97</v>
+      </c>
+      <c r="L543" s="6">
+        <v>108</v>
+      </c>
+      <c r="M543" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N543" s="6">
+        <v>105</v>
+      </c>
+      <c r="O543" s="6">
+        <v>116</v>
+      </c>
+      <c r="P543" s="6"/>
+      <c r="Q543" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R543" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="S543" s="6"/>
+      <c r="T543" s="6"/>
+      <c r="U543" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="544" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A544" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B544" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C544" s="7">
+        <v>1</v>
+      </c>
+      <c r="D544" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E544" s="6">
+        <v>93</v>
+      </c>
+      <c r="F544" s="6">
+        <v>110</v>
+      </c>
+      <c r="G544" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H544" s="6">
+        <v>101</v>
+      </c>
+      <c r="I544" s="6">
+        <v>118</v>
+      </c>
+      <c r="J544" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K544" s="6">
+        <v>77</v>
+      </c>
+      <c r="L544" s="6">
+        <v>134</v>
+      </c>
+      <c r="M544" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N544" s="6">
+        <v>85</v>
+      </c>
+      <c r="O544" s="6">
+        <v>142</v>
+      </c>
+      <c r="P544" s="6"/>
+      <c r="Q544" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R544" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="S544" s="6"/>
+      <c r="T544" s="6"/>
+      <c r="U544" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="545" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A545" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B545" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C545" s="7">
+        <v>1</v>
+      </c>
+      <c r="D545" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E545" s="6">
+        <v>93</v>
+      </c>
+      <c r="F545" s="6">
+        <v>110</v>
+      </c>
+      <c r="G545" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H545" s="6">
+        <v>101</v>
+      </c>
+      <c r="I545" s="6">
+        <v>118</v>
+      </c>
+      <c r="J545" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K545" s="6">
+        <v>97</v>
+      </c>
+      <c r="L545" s="6">
+        <v>108</v>
+      </c>
+      <c r="M545" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N545" s="6">
+        <v>105</v>
+      </c>
+      <c r="O545" s="6">
+        <v>116</v>
+      </c>
+      <c r="P545" s="6"/>
+      <c r="Q545" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R545" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="S545" s="6"/>
+      <c r="T545" s="6"/>
+      <c r="U545" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="546" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A546" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B546" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C546" s="7">
+        <v>1</v>
+      </c>
+      <c r="D546" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E546" s="6">
+        <v>93</v>
+      </c>
+      <c r="F546" s="6">
+        <v>110</v>
+      </c>
+      <c r="G546" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H546" s="6">
+        <v>101</v>
+      </c>
+      <c r="I546" s="6">
+        <v>118</v>
+      </c>
+      <c r="J546" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K546" s="6">
+        <v>77</v>
+      </c>
+      <c r="L546" s="6">
+        <v>134</v>
+      </c>
+      <c r="M546" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N546" s="6">
+        <v>85</v>
+      </c>
+      <c r="O546" s="6">
+        <v>142</v>
+      </c>
+      <c r="P546" s="6"/>
+      <c r="Q546" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="R546" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="S546" s="6"/>
+      <c r="T546" s="6"/>
+      <c r="U546" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="547" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A547" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B547" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C547" s="7">
+        <v>1</v>
+      </c>
+      <c r="D547" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E547" s="6">
+        <v>83</v>
+      </c>
+      <c r="F547" s="6">
+        <v>92</v>
+      </c>
+      <c r="G547" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H547" s="6">
+        <v>91</v>
+      </c>
+      <c r="I547" s="6">
+        <v>100</v>
+      </c>
+      <c r="J547" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K547" s="6">
+        <v>77</v>
+      </c>
+      <c r="L547" s="6">
+        <v>134</v>
+      </c>
+      <c r="M547" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N547" s="6">
+        <v>85</v>
+      </c>
+      <c r="O547" s="6">
+        <v>142</v>
+      </c>
+      <c r="P547" s="6"/>
+      <c r="Q547" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="R547" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="S547" s="6"/>
+      <c r="T547" s="6"/>
+      <c r="U547" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="548" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A548" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B548" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C548" s="7">
+        <v>1</v>
+      </c>
+      <c r="D548" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E548" s="6">
+        <v>83</v>
+      </c>
+      <c r="F548" s="6">
+        <v>92</v>
+      </c>
+      <c r="G548" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H548" s="6">
+        <v>91</v>
+      </c>
+      <c r="I548" s="6">
+        <v>100</v>
+      </c>
+      <c r="J548" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K548" s="6">
+        <v>77</v>
+      </c>
+      <c r="L548" s="6">
+        <v>134</v>
+      </c>
+      <c r="M548" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N548" s="6">
+        <v>85</v>
+      </c>
+      <c r="O548" s="6">
+        <v>142</v>
+      </c>
+      <c r="P548" s="6"/>
+      <c r="Q548" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="R548" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="S548" s="6"/>
+      <c r="T548" s="6"/>
+      <c r="U548" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="549" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A549" s="6"/>
+      <c r="B549" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C549" s="7">
+        <v>1</v>
+      </c>
+      <c r="D549" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E549" s="6">
+        <v>3</v>
+      </c>
+      <c r="F549" s="6">
+        <v>12</v>
+      </c>
+      <c r="G549" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H549" s="6">
+        <v>25</v>
+      </c>
+      <c r="I549" s="6">
+        <v>34</v>
+      </c>
+      <c r="J549" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="K549" s="6">
+        <v>3</v>
+      </c>
+      <c r="L549" s="6">
+        <v>11</v>
+      </c>
+      <c r="M549" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="N549" s="6">
+        <v>25</v>
+      </c>
+      <c r="O549" s="6">
+        <v>33</v>
+      </c>
+      <c r="P549" s="6"/>
+      <c r="Q549" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="R549" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="S549" s="6"/>
+      <c r="T549" s="6"/>
+      <c r="U549" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="550" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A550" s="6"/>
+      <c r="B550" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C550" s="7">
+        <v>1</v>
+      </c>
+      <c r="D550" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E550" s="6">
+        <v>11</v>
+      </c>
+      <c r="F550" s="6">
+        <v>21</v>
+      </c>
+      <c r="G550" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H550" s="6">
+        <v>44</v>
+      </c>
+      <c r="I550" s="6">
+        <v>54</v>
+      </c>
+      <c r="J550" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K550" s="6">
+        <v>11</v>
+      </c>
+      <c r="L550" s="6">
+        <v>20</v>
+      </c>
+      <c r="M550" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="N550" s="6">
+        <v>44</v>
+      </c>
+      <c r="O550" s="6">
+        <v>53</v>
+      </c>
+      <c r="P550" s="6"/>
+      <c r="Q550" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="R550" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="S550" s="6"/>
+      <c r="T550" s="6"/>
+      <c r="U550" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1:V14">
+  <sortState ref="A2:V529">
     <sortCondition ref="E1:E14"/>
     <sortCondition ref="F1:F14"/>
     <sortCondition ref="H1:H14"/>
@@ -36933,6 +38007,11 @@
     <sortCondition ref="N1:N14"/>
     <sortCondition ref="O1:O14"/>
   </sortState>
+  <conditionalFormatting sqref="AH533:AH550">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>